<commit_message>
Add figures for presentation; iterate on figures
</commit_message>
<xml_diff>
--- a/ALLDATA.xlsx
+++ b/ALLDATA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jocelynreahl/Documents/BergmannLab_2018-2020/Reahl_2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BF61AD-5059-2F42-8C6C-D7C7996F16B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33317FBC-E738-314E-8834-03796E660C98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="440" windowWidth="25540" windowHeight="14180" xr2:uid="{75335D1A-4D0E-7A45-9BB4-AFE682FEF120}"/>
   </bookViews>
@@ -1122,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBD3977-3B25-2B4B-A12F-BC2813C3D4A5}">
   <dimension ref="A1:AD123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G120" sqref="G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12195,7 +12195,7 @@
         <v>209</v>
       </c>
       <c r="F121" t="s">
-        <v>205</v>
+        <v>226</v>
       </c>
       <c r="G121" t="s">
         <v>156</v>

</xml_diff>

<commit_message>
Edit Heatmap after F/G reorganization
</commit_message>
<xml_diff>
--- a/ALLDATA.xlsx
+++ b/ALLDATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jocelynreahl/Documents/BergmannLab_2018-2020/Reahl_2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04218B4-076C-3043-9503-A059A3A70B06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9254D6-2053-864C-92CD-A71C4D754B43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="440" windowWidth="25540" windowHeight="14180" xr2:uid="{75335D1A-4D0E-7A45-9BB4-AFE682FEF120}"/>
   </bookViews>
@@ -1129,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBD3977-3B25-2B4B-A12F-BC2813C3D4A5}">
   <dimension ref="A1:AE117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7251,7 +7251,7 @@
         <v>169</v>
       </c>
       <c r="I65" s="19">
-        <v>89.24</v>
+        <v>98.24</v>
       </c>
       <c r="J65" s="7">
         <v>1</v>

</xml_diff>